<commit_message>
Signed-off-by: Robert Sheehy <ms0036625@mtu.ie>
</commit_message>
<xml_diff>
--- a/3D Matrix transformations.xlsx
+++ b/3D Matrix transformations.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS0036625\Documents\CG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS0036625\Desktop\CG25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4100E9D-90A5-4F93-9237-5227E40E08ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A927413A-3E4E-4CDC-A93F-7A02646D98BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -73,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,22 +210,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,34 +324,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.17320508075688773</c:v>
+                  <c:v>-162.05282310692752</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>1.0123407031965235</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.96342366258080214</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.12200846792814624</c:v>
+                  <c:v>1.0374905145595645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.18301270189221935</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.16666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.16666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.25</c:v>
+                  <c:v>-0.98765927360317796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,34 +348,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.24641016151377548</c:v>
+                  <c:v>13130.558738459951</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.024989822151219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-1.0000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.16666666666666666</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.24999999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.97561944361674624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -545,6 +517,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -552,7 +525,323 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$45:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-162.05282310692752</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0123407031965235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.96342366258080214</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0374905145595645</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.98765927360317796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$45:$G$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13130.558738459951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.024989822151219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97561944361674624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B442-4A1D-B778-2184CE7156DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="471982960"/>
+        <c:axId val="471983440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="471982960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471983440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="471983440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471982960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -627,7 +916,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1191,16 +2036,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>430530</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>35379</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>580753</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>96338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1220,6 +2065,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>488674</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>44726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>120926</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5F21D2-39E8-B2F0-AFBC-3E4861FB5DAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1545,42 +2426,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.796875" style="1"/>
-    <col min="6" max="7" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="8.796875" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="7" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1">
         <f>RADIANS(B1)</f>
-        <v>0.52359877559829882</v>
+        <v>1.7453292519943295E-2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1591,25 +2472,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
         <v>1</v>
       </c>
       <c r="F3" s="1">
         <f>SQRT(B3*B3+C3*C3+D3*D3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1619,73 +2500,73 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:D4" si="0">C3/$F$3</f>
-        <v>0</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="F4" s="1">
         <f>SQRT(B4*B4+C4*C4+D4*D4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.4" thickBot="1"/>
-    <row r="8" spans="1:13" ht="14.4" thickTop="1">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6">
         <f>COS(D1)+B4*B4*(1-COS(D1))</f>
-        <v>0.86602540378443871</v>
+        <v>0.99984769515639127</v>
       </c>
       <c r="C8" s="1">
         <f>B4*C4*(1-COS(D1))-D4*SIN(D1)</f>
-        <v>-0.49999999999999994</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="D8" s="1">
         <f>B4*D4*(1-COS(D1)) + C4*SIN(D1)</f>
-        <v>0</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <f>C4*B4*(1-COS(D1)) + D4*SIN(D1)</f>
-        <v>0.49999999999999994</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="C9" s="1">
         <f>COS(D1)+C4*C4*(1-COS(D1))</f>
-        <v>0.86602540378443871</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="D9" s="1">
         <f>C4*D4*(1-COS(D1))-B4*SIN(D1)</f>
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="E9" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <f>D4*B4*(1-COS(D1))-C4*SIN(D1)</f>
-        <v>0</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="C10" s="1">
         <f>D4*C4*(1-COS(D1))+B4*SIN(D1)</f>
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="D10" s="1">
         <f>COS(D1)+D4*D4*(1-COS(D1))</f>
-        <v>1</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.4" thickBot="1">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <v>0</v>
       </c>
@@ -1699,8 +2580,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.4" thickTop="1"/>
-    <row r="13" spans="1:13">
+    <row r="12" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1711,41 +2592,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0</v>
-      </c>
-      <c r="D14" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.4" thickBot="1">
-      <c r="B16" s="14" t="s">
+      <c r="B14" s="12">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14" t="s">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="2:13" ht="14.4" thickTop="1">
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>1</v>
       </c>
@@ -1757,22 +2638,22 @@
       </c>
       <c r="E17" s="7">
         <f>B14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="6">
         <f>B8</f>
-        <v>0.86602540378443871</v>
-      </c>
-      <c r="G17" s="16">
-        <f t="shared" ref="G17:I20" si="1">C8</f>
-        <v>-0.49999999999999994</v>
-      </c>
-      <c r="H17" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="G17" s="1">
+        <f>C8</f>
+        <v>-1.2340714939826924E-2</v>
+      </c>
+      <c r="H17" s="1">
+        <f>D8</f>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="I17" s="7">
-        <f t="shared" si="1"/>
+        <f>E8</f>
         <v>0</v>
       </c>
       <c r="J17" s="6">
@@ -1786,10 +2667,10 @@
       </c>
       <c r="M17" s="7">
         <f>-B14</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>0</v>
       </c>
@@ -1804,19 +2685,19 @@
         <v>0</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" ref="F18:F20" si="2">B9</f>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="G18" s="16">
-        <f t="shared" si="1"/>
-        <v>0.86602540378443871</v>
-      </c>
-      <c r="H18" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="F18:F20" si="1">B9</f>
+        <v>1.2340714939826924E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" ref="G17:I20" si="2">C9</f>
+        <v>0.99992384757819563</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="I18" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="8">
@@ -1833,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>0</v>
       </c>
@@ -1845,22 +2726,22 @@
       </c>
       <c r="E19" s="9">
         <f>D14</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F19" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.2340714939826924E-2</v>
+      </c>
+      <c r="G19" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="16">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7.6152421804365198E-5</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99992384757819563</v>
       </c>
       <c r="I19" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="8">
@@ -1874,10 +2755,10 @@
       </c>
       <c r="M19" s="9">
         <f>-D14</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="14.4" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10">
         <v>0</v>
       </c>
@@ -1891,19 +2772,19 @@
         <v>1</v>
       </c>
       <c r="F20" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="16">
-        <f t="shared" si="1"/>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J20" s="10">
@@ -1919,21 +2800,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="14.4" thickTop="1"/>
-    <row r="22" spans="2:13" ht="14.4" thickBot="1"/>
-    <row r="23" spans="2:13" ht="14.4" thickTop="1">
+    <row r="21" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D23" s="6">
         <f t="array" ref="D23:G26">MMULT(B17:E20,F17:I20)</f>
-        <v>0.86602540378443871</v>
+        <v>0.99984769515639127</v>
       </c>
       <c r="E23" s="1">
-        <v>-0.49999999999999994</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="G23" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="6">
         <f>J17</f>
@@ -1949,18 +2830,18 @@
       </c>
       <c r="K23" s="7">
         <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D24" s="8">
-        <v>0.49999999999999994</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>0.86602540378443871</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="G24" s="9">
         <v>0</v>
@@ -1982,18 +2863,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D25" s="8">
-        <v>0</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="F25" s="1">
-        <v>1</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="G25" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" si="4"/>
@@ -2009,10 +2890,10 @@
       </c>
       <c r="K25" s="9">
         <f t="shared" si="7"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" ht="14.4" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="10">
         <v>0</v>
       </c>
@@ -2042,51 +2923,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="15" thickTop="1" thickBot="1"/>
-    <row r="28" spans="2:13" ht="14.4" thickTop="1">
+    <row r="27" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="F28" s="6">
         <f t="array" ref="F28:I31">MMULT(D23:G26,H23:K26)</f>
-        <v>0.86602540378443871</v>
+        <v>0.99984769515639127</v>
       </c>
       <c r="G28" s="1">
-        <v>-0.49999999999999994</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="I28" s="2">
-        <v>0.13397459621556129</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F29" s="8">
-        <v>0.49999999999999994</v>
+        <v>1.2340714939826924E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>0.86602540378443871</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="I29" s="3">
-        <v>-0.49999999999999994</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F30" s="8">
-        <v>0</v>
+        <v>-1.2340714939826924E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>7.6152421804365198E-5</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0.99992384757819563</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="14.4" thickBot="1">
+    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F31" s="10">
         <v>0</v>
       </c>
@@ -2100,152 +2981,160 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="14.4" thickTop="1"/>
-    <row r="33" spans="1:16">
+    <row r="32" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1">
+    <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="13">
-        <v>0</v>
-      </c>
-      <c r="C35" s="13">
-        <v>1</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13">
+      <c r="B35" s="12">
+        <v>0</v>
+      </c>
+      <c r="C35" s="12">
         <v>-1</v>
       </c>
-      <c r="F35" s="13">
+      <c r="D35" s="12">
         <v>-1</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-    </row>
-    <row r="36" spans="1:16" s="1" customFormat="1">
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+    </row>
+    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="12">
         <v>2</v>
       </c>
-      <c r="C36" s="13">
-        <v>0</v>
-      </c>
-      <c r="D36" s="13">
-        <v>0</v>
-      </c>
-      <c r="E36" s="13">
-        <v>0</v>
-      </c>
-      <c r="F36" s="13">
-        <v>0</v>
-      </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" s="1" customFormat="1">
+      <c r="C36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="E36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+    </row>
+    <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="13">
-        <v>5</v>
-      </c>
-      <c r="C37" s="13">
-        <v>6</v>
-      </c>
-      <c r="D37" s="13">
-        <v>4</v>
-      </c>
-      <c r="E37" s="13">
-        <v>6</v>
-      </c>
-      <c r="F37" s="13">
-        <v>4</v>
-      </c>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-    </row>
-    <row r="38" spans="1:16" s="1" customFormat="1">
+      <c r="B37" s="12">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D37" s="12">
+        <v>1</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
+        <v>-1</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+    </row>
+    <row r="38" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="13">
-        <v>1</v>
-      </c>
-      <c r="C38" s="13">
-        <v>1</v>
-      </c>
-      <c r="D38" s="13">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="B38" s="12">
+        <v>1</v>
+      </c>
+      <c r="C38" s="12">
+        <v>1</v>
+      </c>
+      <c r="D38" s="12">
+        <v>1</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1</v>
+      </c>
+      <c r="F38" s="12">
+        <v>1</v>
+      </c>
+      <c r="G38" s="12">
+        <v>1</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <f t="array" ref="B40:B43">MMULT($F$28:$I$31,B35:B38)</f>
-        <v>-0.8660254037844386</v>
+        <v>-2.4681429879653848E-2</v>
       </c>
       <c r="C40" s="1">
         <f t="array" ref="C40:C43">MMULT($F$28:$I$31,C35:C38)</f>
-        <v>1</v>
+        <v>-0.99984769515639127</v>
       </c>
       <c r="D40" s="1">
         <f t="array" ref="D40:D43">MMULT($F$28:$I$31,D35:D38)</f>
-        <v>1</v>
+        <v>-0.97516626527673744</v>
       </c>
       <c r="E40" s="1">
         <f t="array" ref="E40:E43">MMULT($F$28:$I$31,E35:E38)</f>
-        <v>-0.73205080756887742</v>
+        <v>1.0245291250360451</v>
       </c>
       <c r="F40" s="1">
         <f t="array" ref="F40:F43">MMULT($F$28:$I$31,F35:F38)</f>
-        <v>-0.73205080756887742</v>
+        <v>0.99984769515639127</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2253,21 +3142,21 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <v>1.2320508075688774</v>
+        <v>1.9998476951563913</v>
       </c>
       <c r="C41" s="1">
-        <v>0</v>
+        <v>-1.0123407149398269</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>-1.0121884100962184</v>
       </c>
       <c r="E41" s="1">
-        <v>-0.99999999999999989</v>
+        <v>-0.98750698021656436</v>
       </c>
       <c r="F41" s="1">
-        <v>-0.99999999999999989</v>
+        <v>-0.98765928506017309</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2275,21 +3164,21 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <v>5</v>
+        <v>1.523048436087304E-4</v>
       </c>
       <c r="C42" s="1">
-        <v>6</v>
+        <v>-0.98765928506017309</v>
       </c>
       <c r="D42" s="1">
-        <v>4</v>
+        <v>1.0121884100962182</v>
       </c>
       <c r="E42" s="1">
-        <v>6</v>
+        <v>0.98750698021656436</v>
       </c>
       <c r="F42" s="1">
-        <v>4</v>
+        <v>-1.0123407149398269</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2297,7 +3186,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>1</v>
       </c>
@@ -2319,196 +3208,100 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="45" spans="1:16">
-      <c r="B45" s="17">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
         <f t="array" ref="B45:D49">TRANSPOSE(B40:F42)</f>
-        <v>-0.8660254037844386</v>
-      </c>
-      <c r="C45" s="17">
-        <v>1.2320508075688774</v>
-      </c>
-      <c r="D45" s="17">
-        <v>5</v>
+        <v>-2.4681429879653848E-2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1.9998476951563913</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.523048436087304E-4</v>
       </c>
       <c r="F45" s="1">
         <f>B45/D45</f>
-        <v>-0.17320508075688773</v>
+        <v>-162.05282310692752</v>
       </c>
       <c r="G45" s="1">
         <f>C45/D45</f>
-        <v>0.24641016151377548</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="B46" s="17">
-        <v>1</v>
-      </c>
-      <c r="C46" s="17">
-        <v>0</v>
-      </c>
-      <c r="D46" s="17">
-        <v>6</v>
+        <v>13130.558738459951</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>-0.99984769515639127</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-1.0123407149398269</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-0.98765928506017309</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ref="F46:F54" si="8">B46/D46</f>
-        <v>0.16666666666666666</v>
+        <v>1.0123407031965235</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" ref="G46:G54" si="9">C46/D46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="B47" s="17">
-        <v>1</v>
-      </c>
-      <c r="C47" s="17">
-        <v>0</v>
-      </c>
-      <c r="D47" s="17">
-        <v>4</v>
+        <v>1.024989822151219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>-0.97516626527673744</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-1.0121884100962184</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1.0121884100962182</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="8"/>
-        <v>0.25</v>
+        <v>-0.96342366258080214</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="B48" s="17">
-        <v>-0.73205080756887742</v>
-      </c>
-      <c r="C48" s="17">
-        <v>-0.99999999999999989</v>
-      </c>
-      <c r="D48" s="17">
-        <v>6</v>
+        <v>-1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>1.0245291250360451</v>
+      </c>
+      <c r="C48" s="1">
+        <v>-0.98750698021656436</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.98750698021656436</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="8"/>
-        <v>-0.12200846792814624</v>
+        <v>1.0374905145595645</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="9"/>
-        <v>-0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7">
-      <c r="B49" s="17">
-        <v>-0.73205080756887742</v>
-      </c>
-      <c r="C49" s="17">
-        <v>-0.99999999999999989</v>
-      </c>
-      <c r="D49" s="17">
-        <v>4</v>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="C49" s="1">
+        <v>-0.98765928506017309</v>
+      </c>
+      <c r="D49" s="1">
+        <v>-1.0123407149398269</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="8"/>
-        <v>-0.18301270189221935</v>
+        <v>-0.98765927360317796</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="9"/>
-        <v>-0.24999999999999997</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7">
-      <c r="B50" s="1">
-        <f t="array" ref="B50:D54">TRANSPOSE(B35:F37)</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="1">
-        <v>2</v>
-      </c>
-      <c r="D50" s="1">
-        <v>5</v>
-      </c>
-      <c r="F50" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="1">
-        <f t="shared" si="9"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7">
-      <c r="B51" s="1">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1">
-        <v>6</v>
-      </c>
-      <c r="F51" s="1">
-        <f t="shared" si="8"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G51" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7">
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1">
-        <v>4</v>
-      </c>
-      <c r="F52" s="1">
-        <f t="shared" si="8"/>
-        <v>0.25</v>
-      </c>
-      <c r="G52" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7">
-      <c r="B53" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1">
-        <v>6</v>
-      </c>
-      <c r="F53" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.16666666666666666</v>
-      </c>
-      <c r="G53" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7">
-      <c r="B54" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1">
-        <v>4</v>
-      </c>
-      <c r="F54" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.25</v>
-      </c>
-      <c r="G54" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.97561944361674624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>